<commit_message>
Atualização automática de SAO_PEDRO_DO_SUL.xlsx
</commit_message>
<xml_diff>
--- a/SAO_PEDRO_DO_SUL.xlsx
+++ b/SAO_PEDRO_DO_SUL.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\gera-fichas\Comarcas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{92FC2741-06E8-4D1D-90B3-8836D1696EA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E694591-3377-4F50-8A31-D140478B9550}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1210,7 +1210,7 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 3" xfId="1" xr:uid="{526BEB9C-5A46-43D6-9756-1EF55DFFF3DF}"/>
+    <cellStyle name="Normal 3" xfId="1" xr:uid="{6913F0AA-7BE6-4A5D-B56E-AAADFFC7DA6A}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1240,10 +1240,10 @@
         <xdr:cNvPr id="2" name="Chart1" title="Gráfico">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B8354D90-F07E-4BF5-BA33-E1D181DBFCCA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5C3A0604-272A-4213-9CF8-C10072047DFC}"/>
             </a:ext>
             <a:ext uri="GoogleSheetsCustomDataVersion1">
-              <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="" pictureOfChart="1"/>
+              <go:sheetsCustomData xmlns="" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer" xmlns:go="http://customooxmlschemas.google.com/" pictureOfChart="1"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1281,7 +1281,7 @@
         <xdr:cNvPr id="3" name="Shape 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{35484AB4-3CF3-4608-9AF8-E0FF84F160B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7B996793-7DB0-4F2C-B69B-966EDE90C531}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1344,7 +1344,7 @@
         <xdr:cNvPr id="4" name="Shape 2" title="Desenho">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{93662D3B-6E5F-4FFE-92D4-BA7E88152402}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0408F51-8BE4-497F-9B20-CCBF9E2ACC83}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1363,7 +1363,7 @@
           <xdr:cNvPr id="5" name="Shape 4">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9198B3D7-22A8-FDEF-DD46-EE9DD2501E23}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{88FFE452-6884-7E66-6775-6A2F4850EED0}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1412,7 +1412,7 @@
           <xdr:cNvPr id="6" name="Shape 5">
             <a:extLst>
               <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E3F0515D-7C35-3DBA-3390-BFD87263B305}"/>
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1AA36FC0-1DCC-5213-77E4-084193F56193}"/>
               </a:ext>
             </a:extLst>
           </xdr:cNvPr>
@@ -1431,7 +1431,7 @@
             <xdr:cNvPr id="7" name="Shape 6">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0FC9D732-81F2-DF4E-A071-5E4871708879}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{273CF0CF-9A58-67C7-6969-91BF49A629A7}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1462,7 +1462,7 @@
             <xdr:cNvPr id="8" name="Shape 7">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A6C639E-9B06-58EC-A3C5-C78FB8872F05}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F7CC59B1-92E4-8495-A127-8F300CAEBF5C}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1493,7 +1493,7 @@
             <xdr:cNvPr id="9" name="Shape 8">
               <a:extLst>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{337F256A-1FDD-84CF-AAEB-27F766AC40BB}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{491E31D8-3AF6-942A-F5CA-27BB2ACA2C2D}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1536,7 +1536,7 @@
         <xdr:cNvPr id="10" name="image2.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{74F536D6-9681-4458-9642-0A45071E0413}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0F50F07-667C-4B92-9495-DF9984EDBDAD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1574,7 +1574,7 @@
         <xdr:cNvPr id="11" name="image1.png" title="Imagem">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{403A9C5F-92E5-467C-AEAE-708EC014327B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A9599C89-59A9-4D13-A49D-695A6D687B50}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1617,7 +1617,7 @@
         <xdr:cNvPr id="12" name="Imagem 11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{938C5731-A70E-4BDA-A1AC-F688CCC9C713}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01BEED4D-17DF-4C3C-BD17-561A3EC49790}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1930,7 +1930,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F483AAD8-0A2A-4C82-B584-0639F21B4FB8}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4486913-0E04-4A85-8B56-31FDB8BC9AF4}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>

</xml_diff>